<commit_message>
Added new employee in PIM module
</commit_message>
<xml_diff>
--- a/src/test/resources/TestingFile.xlsx
+++ b/src/test/resources/TestingFile.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5DB9B1-EA9D-4A17-977A-87BFFF7899E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9BB935-1229-4CBA-A3F5-3A83C2B7D5E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="38">
   <si>
     <t>url</t>
   </si>
@@ -113,6 +113,24 @@
   </si>
   <si>
     <t>To test user is able to add employee successfully</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>EmployeeId</t>
+  </si>
+  <si>
+    <t>neelesh</t>
+  </si>
+  <si>
+    <t>khatri</t>
+  </si>
+  <si>
+    <t>neel</t>
   </si>
 </sst>
 </file>
@@ -630,10 +648,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -644,9 +662,12 @@
     <col min="8" max="8" width="40.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="45.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -677,8 +698,17 @@
       <c r="J1" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -709,8 +739,17 @@
       <c r="J2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -741,8 +780,17 @@
       <c r="J3" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -773,8 +821,17 @@
       <c r="J4" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -805,8 +862,17 @@
       <c r="J5" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -835,8 +901,17 @@
         <v>27</v>
       </c>
       <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -866,6 +941,15 @@
       </c>
       <c r="J7" s="4" t="s">
         <v>18</v>
+      </c>
+      <c r="K7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added product store code push
</commit_message>
<xml_diff>
--- a/src/test/resources/TestingFile.xlsx
+++ b/src/test/resources/TestingFile.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732EBA66-EBAA-4148-81F5-C09E24404845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F960E67-DB7D-4634-87FC-A8C3F9F43C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="49">
   <si>
     <t>url</t>
   </si>
@@ -143,6 +143,27 @@
   </si>
   <si>
     <t>To test user is able to update employee detail successfully</t>
+  </si>
+  <si>
+    <t>https://www.demoblaze.com/index.html</t>
+  </si>
+  <si>
+    <t>testSignUp</t>
+  </si>
+  <si>
+    <t>To test user is able to successfully sign up</t>
+  </si>
+  <si>
+    <t>ankitapatel</t>
+  </si>
+  <si>
+    <t>ankita</t>
+  </si>
+  <si>
+    <t>To test use is able to login successfully</t>
+  </si>
+  <si>
+    <t>testLoginProductStore</t>
   </si>
 </sst>
 </file>
@@ -571,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -645,12 +666,40 @@
         <v>40</v>
       </c>
       <c r="B5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7">
         <v>1</v>
       </c>
     </row>
@@ -674,10 +723,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -995,7 +1044,7 @@
         <v>25</v>
       </c>
       <c r="F8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" t="s">
         <v>7</v>
@@ -1016,6 +1065,88 @@
         <v>39</v>
       </c>
       <c r="M8" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>109</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>109</v>
+      </c>
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1045,7 +1176,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
           <x14:formula1>
-            <xm:f>Sheet2!$B$2:$B$2</xm:f>
+            <xm:f>Sheet2!$B$2:$B$3</xm:f>
           </x14:formula1>
           <xm:sqref>E2:E1048576</xm:sqref>
         </x14:dataValidation>
@@ -1060,7 +1191,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1100,6 +1231,9 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
       <c r="C3" t="b">
         <v>0</v>
       </c>

</xml_diff>